<commit_message>
Alteração e adicção de requisitos
</commit_message>
<xml_diff>
--- a/Requisitos/Requisitos Funcionais/requisitosFuncionais.xlsx
+++ b/Requisitos/Requisitos Funcionais/requisitosFuncionais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfeli\Desktop\ProjetoES2\Requisitos\Requisitos Funcionais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E9DE52-538F-4257-9FB8-0486119F221E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C731485-A5ED-41E9-8CCE-6DF16E2C5E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4ABF0B59-3EAA-4472-9014-1459B26A9A3B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t xml:space="preserve">LISTA DE REQUISITOS FUNCIONAIS </t>
   </si>
@@ -90,18 +90,6 @@
     <t>Recuperar senha</t>
   </si>
   <si>
-    <t>Gerenciar usuários</t>
-  </si>
-  <si>
-    <t>Gerenciar estabelecimentos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fazer login aplicação </t>
-  </si>
-  <si>
-    <t>Fazer logout na aplicação</t>
-  </si>
-  <si>
     <t>RF09</t>
   </si>
   <si>
@@ -153,22 +141,49 @@
     <t xml:space="preserve">Este requisito permite a rastreabilidade dos estabelecimentos parceiros. Este requisito cobre a possibilidade de rastrear e manter histórico da localização de um local, usando geolocalização. Opção para usuário Consumidor. </t>
   </si>
   <si>
-    <t xml:space="preserve">Este requisito permite o gerenciamento de parceiros permite o cadastro, alteração e exclusão. O cadastro envolve dados sensíveis, como endereço, tabela de preços etc. Opção para usuário Empresa. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Este requisito permite um filtro de informações como por exemplo: distância dos estabelecimentos, avaliação, preços e etc.Associado com o requisito de localizar estabelecimento </t>
   </si>
   <si>
     <t xml:space="preserve">Este requisito permite lançar informações a respeito da experiência dos usuários, tanto em relação aos locais pesquisados como número de estrelas e alguma descrição. </t>
   </si>
   <si>
-    <t xml:space="preserve">Este requisito permite aos usuários denunciar um perfil de usuário suspeito. O administrador vai gerenciar a penalidade a ser imposta. </t>
-  </si>
-  <si>
     <t>Este requisito permite aos usuários denunciarem perfis comerciais que não estejam com informações corretas. Sendo passível de penalidade</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Gerenciar Conta</t>
+  </si>
+  <si>
+    <t>Este requisito permite que o usuário administrador aprove ou reprove a criação de contas comerciais.</t>
+  </si>
+  <si>
+    <t>Aprovar conta de usuário empresa</t>
+  </si>
+  <si>
+    <t>RF11</t>
+  </si>
+  <si>
+    <t>Esse requisito permite o registro, alteração e exclução de tipos de combustíveis e seus preços para usuários empresa</t>
+  </si>
+  <si>
+    <t>Gerenciar Combustiveis</t>
+  </si>
+  <si>
+    <t>Fazer login</t>
+  </si>
+  <si>
+    <t>Fazer logout</t>
+  </si>
+  <si>
+    <t>Rf12</t>
+  </si>
+  <si>
+    <t>Aprovar denuncia</t>
+  </si>
+  <si>
+    <t>Este requisito permite que o usuário administrador aprove ou reprove denuncias de usuários assim como impor penalidades ao perfil</t>
+  </si>
+  <si>
+    <t>Este requisito permite aos usuários denunciar um perfil de usuário suspeito. É passível de penalidade</t>
   </si>
 </sst>
 </file>
@@ -261,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -277,6 +292,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3837308E-2BE3-4051-9282-618B7392BE50}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,16 +673,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="145.5" x14ac:dyDescent="0.35">
@@ -672,16 +690,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="55.5" x14ac:dyDescent="0.35">
@@ -692,13 +710,13 @@
         <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="109.5" x14ac:dyDescent="0.35">
@@ -706,135 +724,153 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="127.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:5" ht="109.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="109.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:5" ht="91.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="91.5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="73.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
@@ -1059,13 +1095,6 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1077,12 +1106,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D8D8B255028B5643BB55C1A3BFC7FD61" ma:contentTypeVersion="4" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="6735b42515e4ba77a6f0ba9d983f439d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3c7481d6-02b2-49c8-9c78-f7718732c5ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9af0aa5eec320c4cfd5b1a7e2b8b105f" ns2:_="">
     <xsd:import namespace="3c7481d6-02b2-49c8-9c78-f7718732c5ad"/>
@@ -1226,6 +1249,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1236,15 +1265,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75B64359-883D-40D9-AA7F-9025B1F9CEFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B09FA3A-8B7A-413D-8D77-66AA020163B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1262,6 +1282,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75B64359-883D-40D9-AA7F-9025B1F9CEFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6808304-8C27-46DA-A332-33465EEC9CDD}">
   <ds:schemaRefs>

</xml_diff>